<commit_message>
subo cambios temporales sujetos a modificación
</commit_message>
<xml_diff>
--- a/data/choferes.xlsx
+++ b/data/choferes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">id_chofer</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">direccion</t>
   </si>
   <si>
+    <t xml:space="preserve">localidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">disponible</t>
   </si>
   <si>
@@ -43,10 +46,19 @@
     <t xml:space="preserve">Cristina</t>
   </si>
   <si>
-    <t xml:space="preserve">El Pampero 5790, La Matanza </t>
+    <t xml:space="preserve">El Pampero 5790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la matanza</t>
   </si>
   <si>
     <t xml:space="preserve">si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jorge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomas valle 5890</t>
   </si>
 </sst>
 </file>
@@ -145,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,8 +174,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -355,10 +371,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,32 +389,59 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>4</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>